<commit_message>
adicionando opcoes do contrato na interface
</commit_message>
<xml_diff>
--- a/Tabela ponto terceirizados.xlsx
+++ b/Tabela ponto terceirizados.xlsx
@@ -123,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -135,6 +135,20 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -197,11 +211,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -288,9 +302,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>417240</xdr:colOff>
+      <xdr:colOff>416520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>681120</xdr:rowOff>
+      <xdr:rowOff>680400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -304,7 +318,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10440" y="0"/>
-          <a:ext cx="1867320" cy="681120"/>
+          <a:ext cx="1866600" cy="680400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -432,8 +446,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8:G38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
alterando tabela e a função pra centralizar a assinatura e deixar com linhas ao redor da celula
</commit_message>
<xml_diff>
--- a/Tabela ponto terceirizados.xlsx
+++ b/Tabela ponto terceirizados.xlsx
@@ -123,7 +123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -135,20 +135,6 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -178,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +182,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,14 +198,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,9 +284,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>416520</xdr:colOff>
+      <xdr:colOff>415440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>680400</xdr:rowOff>
+      <xdr:rowOff>679320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -318,7 +300,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10440" y="0"/>
-          <a:ext cx="1866600" cy="680400"/>
+          <a:ext cx="1865520" cy="679320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -446,8 +428,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -478,10 +460,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -492,10 +474,10 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -506,10 +488,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
@@ -520,458 +502,458 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="A8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+      <c r="A9" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
+      <c r="A10" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
+      <c r="A11" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="n">
+      <c r="A12" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="n">
+      <c r="A13" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
+      <c r="A14" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="n">
+      <c r="A15" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="n">
+      <c r="A16" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="n">
+      <c r="A17" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="n">
+      <c r="A18" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="n">
+      <c r="A19" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="n">
+      <c r="A20" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="n">
+      <c r="A21" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="n">
+      <c r="A22" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="n">
+      <c r="A23" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="n">
+      <c r="A24" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="n">
+      <c r="A25" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="n">
+      <c r="A26" s="7" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="n">
+      <c r="A27" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="n">
+      <c r="A28" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="n">
+      <c r="A29" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="n">
+      <c r="A30" s="7" t="n">
         <v>23</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="n">
+      <c r="A31" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="n">
+      <c r="A32" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="n">
+      <c r="A33" s="7" t="n">
         <v>26</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="n">
+      <c r="A34" s="7" t="n">
         <v>27</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="n">
+      <c r="A35" s="7" t="n">
         <v>28</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="n">
+      <c r="A36" s="7" t="n">
         <v>29</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="n">
+      <c r="A37" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="n">
+      <c r="A38" s="7" t="n">
         <v>31</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>